<commit_message>
Wareneingangsprotokoll, Emailversand und Link in Übersicht
Im Wareneingangsprotokol wird jetzt der Ursprung und Bemerkung angedruckt
Der Emailversand wurde erweitert um Lager, WaWi und Logistik
In der Übersicht kann mann nicht mehr auf die Detailansicht, die nicht funtioniert.
</commit_message>
<xml_diff>
--- a/application/templates/inboundprotocoll2.xlsx
+++ b/application/templates/inboundprotocoll2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Wareneingangsprotokoll</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Paletten</t>
+  </si>
+  <si>
+    <t>Ursprung</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,21 +585,26 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Beschädigte und verweigerte Ware im WE
</commit_message>
<xml_diff>
--- a/application/templates/inboundprotocoll2.xlsx
+++ b/application/templates/inboundprotocoll2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Wareneingangsprotokoll</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Ursprung</t>
+  </si>
+  <si>
+    <t>Einheiten geprüft:</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I28"/>
+  <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,6 +634,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.24166666666666667" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>